<commit_message>
Add chip area chart to slide deck
</commit_message>
<xml_diff>
--- a/chip_area_bar_charts.xlsx
+++ b/chip_area_bar_charts.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -286,8 +286,8 @@
         </c:dLbls>
         <c:gapWidth val="401"/>
         <c:overlap val="100"/>
-        <c:axId val="1381062976"/>
-        <c:axId val="1378853648"/>
+        <c:axId val="1390112400"/>
+        <c:axId val="1385074128"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -485,11 +485,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1357471696"/>
-        <c:axId val="1380275248"/>
+        <c:axId val="1377986256"/>
+        <c:axId val="1311729840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1381062976"/>
+        <c:axId val="1390112400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -532,7 +532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1378853648"/>
+        <c:crossAx val="1385074128"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -540,7 +540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1378853648"/>
+        <c:axId val="1385074128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45.0"/>
@@ -591,12 +591,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1381062976"/>
+        <c:crossAx val="1390112400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1380275248"/>
+        <c:axId val="1311729840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45.0"/>
@@ -630,12 +630,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1357471696"/>
+        <c:crossAx val="1377986256"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1357471696"/>
+        <c:axId val="1377986256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -645,7 +645,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1380275248"/>
+        <c:crossAx val="1311729840"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>

</xml_diff>